<commit_message>
Scripting DPLKINV001-019, DPLKKPS001-001 until DPLKKPS001-003, Re-run DPLKINV001-009 until DPLKINV001-015, and Update Function Sidebar
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-019 - Setup Profile Bank Investasi - Pasar Uang Tambah, Ubah, View Detil & Hapus Data.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV001-019 - Setup Profile Bank Investasi - Pasar Uang Tambah, Ubah, View Detil & Hapus Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0063CA33-9F0C-44B4-A036-B45AA002E08F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0648B436-C204-4AB8-B0B0-759B586E4C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>SIDEBAR_MENU</t>
   </si>
@@ -190,6 +190,46 @@
   </si>
   <si>
     <t>Verifikasi Profile Bank</t>
+  </si>
+  <si>
+    <t>PAU0268</t>
+  </si>
+  <si>
+    <t>STATUS_VERIFIKASI</t>
+  </si>
+  <si>
+    <t>KETERANGAN_VERIFIKASI</t>
+  </si>
+  <si>
+    <t>0 : Kembalikan ke Data Entry</t>
+  </si>
+  <si>
+    <t>Tolong Diperbaiki</t>
+  </si>
+  <si>
+    <t>Verifikasi Data - Data Dikembalikan Dapat dilakukan dengan baik</t>
+  </si>
+  <si>
+    <t>Verifikasi Data - Data Disetujui Dapat dilakukan dengan baik</t>
+  </si>
+  <si>
+    <t>1 : Setuju</t>
+  </si>
+  <si>
+    <t>Disetujui</t>
+  </si>
+  <si>
+    <t>PAU0271</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Bank ID : PAU0271</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Bank ID : PAU0268</t>
   </si>
   <si>
     <t>Username : Putri;
@@ -209,60 +249,25 @@
 Jenis Perhitungan Bunga : Memperhitungkan Hari Libur;
 Syariah : Checked;
 Tgl. Non Aktif : 18/11/2022;
-Non. Aktif : Checked;</t>
+Non. Aktif : Checked</t>
   </si>
   <si>
     <t>Username : Putri;
 Password : bni1234/;
-Bank ID : PAU0269 (sesuaikan dengan hasil generate);
+Bank ID : PAU0271 (sesuaikan dengan hasil generate);
+Petugas Submit : Putri;
+Tanggal Verifikasi : Tanggal hari ini;
+Status Verifikasi : 0 - Dikembalikan ke Data Entry;
+Keterangan Verifikasi : Tolong Diperbaiki</t>
+  </si>
+  <si>
+    <t>Username : Putri;
+Password : bni1234/;
+Bank ID : PAU0271 (sesuaikan dengan hasil generate);
 Petugas Submit : Putri;
 Tanggal Verifikasi : Tanggal hari ini;
 Status Verifikasi : 1 - Setuju;
-Keterangan Verifikasi w: Disetujui;</t>
-  </si>
-  <si>
-    <t>Username : Putri;
-Password : bni1234/;
-Bank ID : PAU0269</t>
-  </si>
-  <si>
-    <t>PAU0269</t>
-  </si>
-  <si>
-    <t>PAU0268</t>
-  </si>
-  <si>
-    <t>STATUS_VERIFIKASI</t>
-  </si>
-  <si>
-    <t>KETERANGAN_VERIFIKASI</t>
-  </si>
-  <si>
-    <t>0 : Kembalikan ke Data Entry</t>
-  </si>
-  <si>
-    <t>Tolong Diperbaiki</t>
-  </si>
-  <si>
-    <t>Verifikasi Data - Data Dikembalikan Dapat dilakukan dengan baik</t>
-  </si>
-  <si>
-    <t>Verifikasi Data - Data Disetujui Dapat dilakukan dengan baik</t>
-  </si>
-  <si>
-    <t>1 : Setuju</t>
-  </si>
-  <si>
-    <t>Disetujui</t>
-  </si>
-  <si>
-    <t>Username : Putri;
-Password : bni1234/;
-Bank ID : PAU0269 (sesuaikan dengan hasil generate);
-Petugas Submit : Putri;
-Tanggal Verifikasi : Tanggal hari ini;
-Status Verifikasi : 0 - Dikembalikan ke Data Entry;
-Keterangan Verifikasi : Tolong Diperbaiki;</t>
+Keterangan Verifikasi w: Disetujui</t>
   </si>
 </sst>
 </file>
@@ -645,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,10 +774,10 @@
         <v>43</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="300" x14ac:dyDescent="0.25">
@@ -792,7 +797,7 @@
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>10</v>
@@ -813,7 +818,7 @@
         <v>18</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>51</v>
@@ -875,7 +880,7 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>10</v>
@@ -896,7 +901,7 @@
         <v>18</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="5"/>
@@ -921,7 +926,7 @@
         <v>53</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>69</v>
@@ -945,7 +950,7 @@
         <v>55</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="N4" s="6"/>
       <c r="O4" s="3"/>
@@ -957,10 +962,10 @@
       <c r="U4" s="2"/>
       <c r="V4" s="2"/>
       <c r="AC4" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AD4" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:30" ht="45" x14ac:dyDescent="0.25">
@@ -1001,7 +1006,7 @@
         <v>18</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="N5" s="3"/>
       <c r="O5" s="3"/>
@@ -1030,10 +1035,10 @@
         <v>53</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>10</v>
@@ -1054,7 +1059,7 @@
         <v>55</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="3"/>
@@ -1066,10 +1071,10 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="AC6" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="45" x14ac:dyDescent="0.25">
@@ -1089,7 +1094,7 @@
         <v>17</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
@@ -1110,7 +1115,7 @@
         <v>18</v>
       </c>
       <c r="M7" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>